<commit_message>
Uploading ordered rev1 files
</commit_message>
<xml_diff>
--- a/Firefly_V1_Bom.xlsx
+++ b/Firefly_V1_Bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\repos\firefly-led-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACDEACE-05CF-4262-ACB1-CE28604BC30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E022127-A356-45C9-932D-93BBA9CF4891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3915" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{45A1EDE2-A2F3-40DF-ACA1-A39F063FACEE}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Part</t>
   </si>
@@ -108,6 +107,9 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Panasonic/EVQ-9P701P?qs=NPkb10g2yLBKCwpELvsGNg%3D%3D</t>
+  </si>
+  <si>
+    <t>5.1k resistor</t>
   </si>
 </sst>
 </file>
@@ -459,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE805AB9-5B79-4720-899E-7A9AF6DC7B2D}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,6 +611,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>